<commit_message>
megre final de la semana
</commit_message>
<xml_diff>
--- a/P3GA3/Cronograma Y Diagrama Hijo/Cronograma-Grupo3.xlsx
+++ b/P3GA3/Cronograma Y Diagrama Hijo/Cronograma-Grupo3.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Langas\Desktop\Programacion lll\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Langas\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1DD60D3-2766-4F77-BBC7-9995F4F61C41}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42CFB261-F2D0-4E01-8E09-93352B08468A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1669,8 +1669,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1823,7 +1823,7 @@
         <v>16</v>
       </c>
       <c r="G6" s="9">
-        <v>0.9</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="45" x14ac:dyDescent="0.25">
@@ -1847,7 +1847,7 @@
         <v>6</v>
       </c>
       <c r="G7" s="9">
-        <v>0.9</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="45" x14ac:dyDescent="0.25">
@@ -1871,7 +1871,7 @@
         <v>11</v>
       </c>
       <c r="G8" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -1895,7 +1895,7 @@
         <v>11</v>
       </c>
       <c r="G9" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -1919,7 +1919,7 @@
         <v>18</v>
       </c>
       <c r="G10" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -1943,7 +1943,7 @@
         <v>11</v>
       </c>
       <c r="G11" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -1967,7 +1967,7 @@
         <v>16</v>
       </c>
       <c r="G12" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1991,7 +1991,7 @@
         <v>23</v>
       </c>
       <c r="G13" s="9">
-        <v>0.8</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2015,7 +2015,7 @@
         <v>15</v>
       </c>
       <c r="G14" s="9">
-        <v>0</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2039,7 +2039,7 @@
         <v>15</v>
       </c>
       <c r="G15" s="9">
-        <v>0.5</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2063,7 +2063,7 @@
         <v>16</v>
       </c>
       <c r="G16" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2087,7 +2087,7 @@
         <v>11</v>
       </c>
       <c r="G17" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2111,7 +2111,7 @@
         <v>18</v>
       </c>
       <c r="G18" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2135,7 +2135,7 @@
         <v>6</v>
       </c>
       <c r="G19" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Actualizado Con Hoja de Desempeño
</commit_message>
<xml_diff>
--- a/P3GA3/Cronograma Y Diagrama Hijo/Cronograma-Grupo3.xlsx
+++ b/P3GA3/Cronograma Y Diagrama Hijo/Cronograma-Grupo3.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Langas\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Langas\Documents\Laboratorio_GruposD\P3GA3\Cronograma Y Diagrama Hijo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42CFB261-F2D0-4E01-8E09-93352B08468A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CACC6A9D-F97D-40A1-B832-27C3045DDEF5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="41">
   <si>
     <t># Actividad</t>
   </si>
@@ -116,9 +116,6 @@
     <t>Soporte de Mantenimientos de software.</t>
   </si>
   <si>
-    <t>Pull request final</t>
-  </si>
-  <si>
     <t>Pull request Geovani</t>
   </si>
   <si>
@@ -132,6 +129,33 @@
   </si>
   <si>
     <t>Agregar Variables Globales Para Conexión BD</t>
+  </si>
+  <si>
+    <t>Pull request final Parte 1</t>
+  </si>
+  <si>
+    <t>Ingreso de Notas</t>
+  </si>
+  <si>
+    <t>Todos</t>
+  </si>
+  <si>
+    <t>Vista de contraseña</t>
+  </si>
+  <si>
+    <t>Arreglo de Errores</t>
+  </si>
+  <si>
+    <t>Pablo Hernandez</t>
+  </si>
+  <si>
+    <t>Diseño y Programacion Consultas</t>
+  </si>
+  <si>
+    <t>Pull request final Parte 2</t>
+  </si>
+  <si>
+    <t>Validaciones de Facultades con Carreras</t>
   </si>
 </sst>
 </file>
@@ -142,8 +166,16 @@
     <numFmt numFmtId="164" formatCode="dd\-mm\-yy;@"/>
     <numFmt numFmtId="165" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
   </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -211,7 +243,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -267,6 +299,9 @@
     <xf numFmtId="165" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="21" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="16" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -433,7 +468,7 @@
                   <c:v>Pul request Pablo</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>Pull request final</c:v>
+                  <c:v>Pull request final Parte 1</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -577,7 +612,7 @@
                   <c:v>Pul request Pablo</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>Pull request final</c:v>
+                  <c:v>Pull request final Parte 1</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1667,10 +1702,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G61"/>
+  <dimension ref="A1:H63"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1694,7 +1729,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E1" s="3" t="s">
         <v>3</v>
@@ -1855,7 +1890,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C8" s="23">
         <v>43963.458333333336</v>
@@ -2047,7 +2082,7 @@
         <v>15</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C16" s="23">
         <v>43964.0625</v>
@@ -2066,12 +2101,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="5">
         <v>16</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C17" s="23">
         <v>43964.083333333336</v>
@@ -2090,12 +2125,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="5">
         <v>17</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C18" s="23">
         <v>43964.104166666664</v>
@@ -2114,12 +2149,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="5">
         <v>18</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="C19" s="23">
         <v>43964.125</v>
@@ -2138,79 +2173,170 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="5"/>
-      <c r="B20" s="6"/>
-      <c r="C20" s="7"/>
-      <c r="D20" s="7"/>
-      <c r="E20" s="7"/>
-      <c r="F20" s="7"/>
-      <c r="G20" s="7"/>
-    </row>
-    <row r="21" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="5"/>
-      <c r="B21" s="6"/>
-      <c r="C21" s="7"/>
-      <c r="D21" s="7"/>
-      <c r="E21" s="7"/>
-      <c r="F21" s="7"/>
-      <c r="G21" s="7"/>
-    </row>
-    <row r="22" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="5"/>
-      <c r="B22" s="6"/>
-      <c r="C22" s="7"/>
-      <c r="D22" s="7"/>
-      <c r="E22" s="7"/>
-      <c r="F22" s="7"/>
-      <c r="G22" s="7"/>
-    </row>
-    <row r="23" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="5"/>
-      <c r="B23" s="6"/>
-      <c r="C23" s="7"/>
-      <c r="D23" s="7"/>
-      <c r="E23" s="7"/>
-      <c r="F23" s="7"/>
-      <c r="G23" s="7"/>
-    </row>
-    <row r="24" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="5"/>
-      <c r="B24" s="6"/>
-      <c r="C24" s="7"/>
-      <c r="D24" s="7"/>
-      <c r="E24" s="7"/>
-      <c r="F24" s="7"/>
-      <c r="G24" s="7"/>
-    </row>
-    <row r="25" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="5"/>
-      <c r="B25" s="6"/>
-      <c r="C25" s="7"/>
-      <c r="D25" s="7"/>
-      <c r="E25" s="7"/>
-      <c r="F25" s="7"/>
-      <c r="G25" s="7"/>
-    </row>
-    <row r="26" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="13"/>
-      <c r="B26" s="14"/>
-      <c r="C26" s="15"/>
-      <c r="D26" s="15"/>
-      <c r="E26" s="15"/>
-      <c r="F26" s="15"/>
-      <c r="G26" s="15"/>
-    </row>
-    <row r="27" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="13"/>
-      <c r="B27" s="14"/>
-      <c r="C27" s="15"/>
-      <c r="D27" s="15"/>
-      <c r="E27" s="15"/>
-      <c r="F27" s="15"/>
-      <c r="G27" s="15"/>
-    </row>
-    <row r="28" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="5">
+        <v>19</v>
+      </c>
+      <c r="B20" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="C20" s="7">
+        <v>43970.125</v>
+      </c>
+      <c r="D20" s="25">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="E20" s="7">
+        <f>C20+D20</f>
+        <v>43970.166666666664</v>
+      </c>
+      <c r="F20" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="G20" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="5">
+        <v>20</v>
+      </c>
+      <c r="B21" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="C21" s="7">
+        <v>43964</v>
+      </c>
+      <c r="D21" s="25">
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="E21" s="7">
+        <f>C21+D21</f>
+        <v>43964.083333333336</v>
+      </c>
+      <c r="F21" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="G21" s="9">
+        <v>1</v>
+      </c>
+      <c r="H21" s="27"/>
+    </row>
+    <row r="22" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="5">
+        <v>21</v>
+      </c>
+      <c r="B22" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="C22" s="7">
+        <v>43970.125</v>
+      </c>
+      <c r="D22" s="25">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="E22" s="7">
+        <f>C22+D22</f>
+        <v>43970.166666666664</v>
+      </c>
+      <c r="F22" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="G22" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="5">
+        <v>22</v>
+      </c>
+      <c r="B23" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="C23" s="7">
+        <v>43966</v>
+      </c>
+      <c r="D23" s="25">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="E23" s="7">
+        <f>C23+D23</f>
+        <v>43966.041666666664</v>
+      </c>
+      <c r="F23" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="G23" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="5">
+        <v>23</v>
+      </c>
+      <c r="B24" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="C24" s="7">
+        <v>43971</v>
+      </c>
+      <c r="D24" s="25">
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="E24" s="7">
+        <f>C24+D24</f>
+        <v>43971.083333333336</v>
+      </c>
+      <c r="F24" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="G24" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="5">
+        <v>23</v>
+      </c>
+      <c r="B25" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="C25" s="7">
+        <v>43972</v>
+      </c>
+      <c r="D25" s="25">
+        <v>1.0416666666666666E-2</v>
+      </c>
+      <c r="E25" s="7">
+        <f>C25+D25</f>
+        <v>43972.010416666664</v>
+      </c>
+      <c r="F25" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="G25" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="5"/>
+      <c r="B26" s="6"/>
+      <c r="C26" s="7"/>
+      <c r="D26" s="7"/>
+      <c r="E26" s="7"/>
+      <c r="F26" s="7"/>
+      <c r="G26" s="26"/>
+    </row>
+    <row r="27" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="5"/>
+      <c r="B27" s="6"/>
+      <c r="C27" s="7"/>
+      <c r="D27" s="7"/>
+      <c r="E27" s="7"/>
+      <c r="F27" s="7"/>
+      <c r="G27" s="7"/>
+    </row>
+    <row r="28" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="13"/>
       <c r="B28" s="14"/>
       <c r="C28" s="15"/>
@@ -2219,7 +2345,7 @@
       <c r="F28" s="15"/>
       <c r="G28" s="15"/>
     </row>
-    <row r="29" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="13"/>
       <c r="B29" s="14"/>
       <c r="C29" s="15"/>
@@ -2228,7 +2354,7 @@
       <c r="F29" s="15"/>
       <c r="G29" s="15"/>
     </row>
-    <row r="30" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="13"/>
       <c r="B30" s="14"/>
       <c r="C30" s="15"/>
@@ -2237,7 +2363,7 @@
       <c r="F30" s="15"/>
       <c r="G30" s="15"/>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="13"/>
       <c r="B31" s="14"/>
       <c r="C31" s="15"/>
@@ -2246,7 +2372,7 @@
       <c r="F31" s="15"/>
       <c r="G31" s="15"/>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="13"/>
       <c r="B32" s="14"/>
       <c r="C32" s="15"/>
@@ -2337,67 +2463,67 @@
       <c r="G41" s="15"/>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A42" s="16"/>
-      <c r="B42" s="17"/>
-      <c r="C42" s="18"/>
-      <c r="D42" s="18"/>
-      <c r="E42" s="18"/>
-      <c r="F42" s="18"/>
-      <c r="G42" s="18"/>
+      <c r="A42" s="13"/>
+      <c r="B42" s="14"/>
+      <c r="C42" s="15"/>
+      <c r="D42" s="15"/>
+      <c r="E42" s="15"/>
+      <c r="F42" s="15"/>
+      <c r="G42" s="15"/>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A43" s="19"/>
-      <c r="B43" s="20"/>
-      <c r="C43" s="21"/>
-      <c r="D43" s="21"/>
-      <c r="E43" s="21"/>
-      <c r="F43" s="21"/>
-      <c r="G43" s="21"/>
-    </row>
-    <row r="44" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A44" s="19"/>
-      <c r="C44" s="12" t="s">
+      <c r="A43" s="13"/>
+      <c r="B43" s="14"/>
+      <c r="C43" s="15"/>
+      <c r="D43" s="15"/>
+      <c r="E43" s="15"/>
+      <c r="F43" s="15"/>
+      <c r="G43" s="15"/>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A44" s="16"/>
+      <c r="B44" s="17"/>
+      <c r="C44" s="18"/>
+      <c r="D44" s="18"/>
+      <c r="E44" s="18"/>
+      <c r="F44" s="18"/>
+      <c r="G44" s="18"/>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A45" s="19"/>
+      <c r="B45" s="20"/>
+      <c r="C45" s="21"/>
+      <c r="D45" s="21"/>
+      <c r="E45" s="21"/>
+      <c r="F45" s="21"/>
+      <c r="G45" s="21"/>
+    </row>
+    <row r="46" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A46" s="19"/>
+      <c r="C46" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="D44" s="24">
+      <c r="D46" s="24">
         <f>C2</f>
         <v>43963.444444444445</v>
       </c>
-      <c r="F44" s="21"/>
-      <c r="G44" s="21"/>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A45" s="19"/>
-      <c r="C45" s="12" t="s">
+      <c r="F46" s="21"/>
+      <c r="G46" s="21"/>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A47" s="19"/>
+      <c r="C47" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="D45" s="24">
+      <c r="D47" s="24">
         <f>E19</f>
         <v>43964.145833333336</v>
       </c>
-      <c r="F45" s="21"/>
-      <c r="G45" s="21"/>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A46" s="19"/>
-      <c r="F46" s="21"/>
-      <c r="G46" s="21"/>
-    </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A47" s="19"/>
-      <c r="B47" s="20"/>
-      <c r="C47" s="21"/>
-      <c r="D47" s="21"/>
-      <c r="E47" s="21"/>
       <c r="F47" s="21"/>
       <c r="G47" s="21"/>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" s="19"/>
-      <c r="B48" s="20"/>
-      <c r="C48" s="21"/>
-      <c r="D48" s="21"/>
-      <c r="E48" s="21"/>
       <c r="F48" s="21"/>
       <c r="G48" s="21"/>
     </row>
@@ -2518,6 +2644,24 @@
       <c r="F61" s="21"/>
       <c r="G61" s="21"/>
     </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A62" s="19"/>
+      <c r="B62" s="20"/>
+      <c r="C62" s="21"/>
+      <c r="D62" s="21"/>
+      <c r="E62" s="21"/>
+      <c r="F62" s="21"/>
+      <c r="G62" s="21"/>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A63" s="19"/>
+      <c r="B63" s="20"/>
+      <c r="C63" s="21"/>
+      <c r="D63" s="21"/>
+      <c r="E63" s="21"/>
+      <c r="F63" s="21"/>
+      <c r="G63" s="21"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
actualizacion cronograma e informe
</commit_message>
<xml_diff>
--- a/P3GA3/Cronograma Y Diagrama Hijo/Cronograma-Grupo3.xlsx
+++ b/P3GA3/Cronograma Y Diagrama Hijo/Cronograma-Grupo3.xlsx
@@ -2,10 +2,10 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ranbr\Documents\programacion3\grupoaleatorio\P3GA3\Cronograma Y Diagrama Hijo\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Geovani\Desktop\LABORATORIO12MAYO\P3GA3\Cronograma Y Diagrama Hijo\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -172,7 +172,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="dd\-mm\-yy;@"/>
     <numFmt numFmtId="165" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
@@ -352,7 +352,7 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="es-ES"/>
   <c:roundedCorners val="0"/>
@@ -569,7 +569,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-FCA0-4202-A4BE-FBB4EAE661C8}"/>
             </c:ext>
@@ -713,7 +713,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+          <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-FCA0-4202-A4BE-FBB4EAE661C8}"/>
             </c:ext>
@@ -1451,7 +1451,7 @@
         <xdr:cNvPr id="3" name="Gráfico 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000003000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1735,10 +1735,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Hoja1"/>
   <dimension ref="A1:I66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="I29" sqref="I29"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="I33" sqref="I33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2096,7 +2097,7 @@
         <v>15</v>
       </c>
       <c r="G14" s="9">
-        <v>0.3</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2298,7 +2299,7 @@
         <v>34</v>
       </c>
       <c r="G22" s="9">
-        <v>0.75</v>
+        <v>0.9</v>
       </c>
       <c r="H22" s="27"/>
     </row>
@@ -2324,7 +2325,7 @@
         <v>16</v>
       </c>
       <c r="G23" s="9">
-        <v>0.9</v>
+        <v>1</v>
       </c>
     </row>
     <row r="24" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2349,7 +2350,7 @@
         <v>40</v>
       </c>
       <c r="G24" s="29">
-        <v>0.3</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="25" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2374,7 +2375,7 @@
         <v>40</v>
       </c>
       <c r="G25" s="29">
-        <v>0.9</v>
+        <v>1</v>
       </c>
     </row>
     <row r="26" spans="1:9" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2399,7 +2400,7 @@
         <v>6</v>
       </c>
       <c r="G26" s="9">
-        <v>0.9</v>
+        <v>1</v>
       </c>
     </row>
     <row r="27" spans="1:9" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2423,7 +2424,7 @@
         <v>6</v>
       </c>
       <c r="G27" s="9">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="28" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -2451,7 +2452,7 @@
       </c>
       <c r="I28" s="31">
         <f>AVERAGE(G2:G28)</f>
-        <v>0.83518518518518503</v>
+        <v>0.92592592592592593</v>
       </c>
     </row>
     <row r="29" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>